<commit_message>
updated the TestData.xlsx excel sheet
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivkumarj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivkumarj\eclipse-workspace\WiproAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3D40A9-340D-47D4-A223-8759F17C5D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12A8CF0-02AE-4A4D-B6BD-A1FD89774052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product to search" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>product to search</t>
   </si>
@@ -37,6 +38,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>expected card value on icon</t>
   </si>
 </sst>
 </file>
@@ -363,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,8 +394,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651ED2EE-C1CB-4A23-A35B-4E641DBCCCC0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>